<commit_message>
fully fucntional CO2 objective
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>element</t>
   </si>
@@ -25,31 +25,16 @@
     <t>demand1</t>
   </si>
   <si>
-    <t>demand2</t>
-  </si>
-  <si>
     <t>net1</t>
   </si>
   <si>
-    <t>net2</t>
-  </si>
-  <si>
     <t>pv1</t>
   </si>
   <si>
-    <t>pv2</t>
-  </si>
-  <si>
     <t>bat1</t>
   </si>
   <si>
-    <t>bat2</t>
-  </si>
-  <si>
     <t>CHP1</t>
-  </si>
-  <si>
-    <t>CHP2</t>
   </si>
   <si>
     <t>demand</t>
@@ -422,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -449,7 +434,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -457,7 +442,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -465,7 +450,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -473,47 +458,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
         <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
with solar_th and pvt
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>element</t>
   </si>
@@ -37,6 +37,12 @@
     <t>CHP1</t>
   </si>
   <si>
+    <t>solar_th1</t>
+  </si>
+  <si>
+    <t>pvt1</t>
+  </si>
+  <si>
     <t>demand</t>
   </si>
   <si>
@@ -50,6 +56,12 @@
   </si>
   <si>
     <t>CHP</t>
+  </si>
+  <si>
+    <t>solar_th</t>
+  </si>
+  <si>
+    <t>pvt</t>
   </si>
 </sst>
 </file>
@@ -407,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,7 +438,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -434,7 +446,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -442,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -450,7 +462,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -458,7 +470,23 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully operating charging station
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>element</t>
   </si>
@@ -31,6 +31,9 @@
     <t>pv1</t>
   </si>
   <si>
+    <t>bat1</t>
+  </si>
+  <si>
     <t>charging_station1</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t>pv</t>
+  </si>
+  <si>
+    <t>bat</t>
   </si>
   <si>
     <t>charging_station</t>
@@ -401,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -428,7 +434,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -436,7 +442,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -444,7 +450,15 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
objective function working with charging station
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>element</t>
   </si>
@@ -34,9 +34,21 @@
     <t>bat1</t>
   </si>
   <si>
+    <t>CHP1</t>
+  </si>
+  <si>
+    <t>solar_th1</t>
+  </si>
+  <si>
+    <t>pvt1</t>
+  </si>
+  <si>
     <t>charging_station1</t>
   </si>
   <si>
+    <t>charging_station2</t>
+  </si>
+  <si>
     <t>demand</t>
   </si>
   <si>
@@ -47,6 +59,15 @@
   </si>
   <si>
     <t>bat</t>
+  </si>
+  <si>
+    <t>CHP</t>
+  </si>
+  <si>
+    <t>solar_th</t>
+  </si>
+  <si>
+    <t>pvt</t>
   </si>
   <si>
     <t>charging_station</t>
@@ -407,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,7 +447,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -434,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -442,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -450,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -458,7 +479,39 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
with heat pump functioning
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>element</t>
   </si>
@@ -34,19 +34,13 @@
     <t>bat1</t>
   </si>
   <si>
-    <t>CHP1</t>
-  </si>
-  <si>
-    <t>solar_th1</t>
-  </si>
-  <si>
     <t>pvt1</t>
   </si>
   <si>
     <t>charging_station1</t>
   </si>
   <si>
-    <t>charging_station2</t>
+    <t>heat_pump1</t>
   </si>
   <si>
     <t>demand</t>
@@ -61,16 +55,13 @@
     <t>bat</t>
   </si>
   <si>
-    <t>CHP</t>
-  </si>
-  <si>
-    <t>solar_th</t>
-  </si>
-  <si>
     <t>pvt</t>
   </si>
   <si>
     <t>charging_station</t>
+  </si>
+  <si>
+    <t>heat_pump</t>
   </si>
 </sst>
 </file>
@@ -428,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,7 +438,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -455,7 +446,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -463,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -471,7 +462,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -479,7 +470,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -487,7 +478,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -495,23 +486,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
failed attempt receding horizon
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>element</t>
   </si>
@@ -34,24 +34,6 @@
     <t>bat1</t>
   </si>
   <si>
-    <t>CHP1</t>
-  </si>
-  <si>
-    <t>solar_th1</t>
-  </si>
-  <si>
-    <t>pvt1</t>
-  </si>
-  <si>
-    <t>charging_station1</t>
-  </si>
-  <si>
-    <t>charging_station2</t>
-  </si>
-  <si>
-    <t>heat_pump1</t>
-  </si>
-  <si>
     <t>demand</t>
   </si>
   <si>
@@ -62,21 +44,6 @@
   </si>
   <si>
     <t>bat</t>
-  </si>
-  <si>
-    <t>CHP</t>
-  </si>
-  <si>
-    <t>solar_th</t>
-  </si>
-  <si>
-    <t>pvt</t>
-  </si>
-  <si>
-    <t>charging_station</t>
-  </si>
-  <si>
-    <t>heat_pump</t>
   </si>
 </sst>
 </file>
@@ -434,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -461,7 +428,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -469,7 +436,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -477,55 +444,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before starting to change charging station
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>element</t>
   </si>
@@ -28,10 +28,7 @@
     <t>net1</t>
   </si>
   <si>
-    <t>pv1</t>
-  </si>
-  <si>
-    <t>bat1</t>
+    <t>charging_station1</t>
   </si>
   <si>
     <t>demand</t>
@@ -40,10 +37,7 @@
     <t>net</t>
   </si>
   <si>
-    <t>pv</t>
-  </si>
-  <si>
-    <t>bat</t>
+    <t>charging_station</t>
   </si>
 </sst>
 </file>
@@ -401,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,7 +414,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -428,7 +422,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -436,15 +430,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
problems with constraint from bat
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>element</t>
   </si>
@@ -25,10 +25,16 @@
     <t>demand1</t>
   </si>
   <si>
+    <t>demand2</t>
+  </si>
+  <si>
     <t>net1</t>
   </si>
   <si>
-    <t>charging_station1</t>
+    <t>pv1</t>
+  </si>
+  <si>
+    <t>bat1</t>
   </si>
   <si>
     <t>demand</t>
@@ -37,7 +43,10 @@
     <t>net</t>
   </si>
   <si>
-    <t>charging_station</t>
+    <t>pv</t>
+  </si>
+  <si>
+    <t>bat</t>
   </si>
 </sst>
 </file>
@@ -395,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +423,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -422,7 +431,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -430,7 +439,23 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting before merging to main
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>element</t>
   </si>
@@ -25,57 +25,15 @@
     <t>demand1</t>
   </si>
   <si>
-    <t>demand2</t>
-  </si>
-  <si>
     <t>net1</t>
   </si>
   <si>
-    <t>net2</t>
-  </si>
-  <si>
     <t>pv1</t>
   </si>
   <si>
-    <t>pv2</t>
-  </si>
-  <si>
     <t>bat1</t>
   </si>
   <si>
-    <t>bat2</t>
-  </si>
-  <si>
-    <t>CHP1</t>
-  </si>
-  <si>
-    <t>CHP2</t>
-  </si>
-  <si>
-    <t>solar_th1</t>
-  </si>
-  <si>
-    <t>solar_th2</t>
-  </si>
-  <si>
-    <t>pvt1</t>
-  </si>
-  <si>
-    <t>pvt2</t>
-  </si>
-  <si>
-    <t>charging_station1</t>
-  </si>
-  <si>
-    <t>charging_station2</t>
-  </si>
-  <si>
-    <t>heat_pump1</t>
-  </si>
-  <si>
-    <t>heat_pump2</t>
-  </si>
-  <si>
     <t>demand</t>
   </si>
   <si>
@@ -86,21 +44,6 @@
   </si>
   <si>
     <t>bat</t>
-  </si>
-  <si>
-    <t>CHP</t>
-  </si>
-  <si>
-    <t>solar_th</t>
-  </si>
-  <si>
-    <t>pvt</t>
-  </si>
-  <si>
-    <t>charging_station</t>
-  </si>
-  <si>
-    <t>heat_pump</t>
   </si>
 </sst>
 </file>
@@ -458,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -485,7 +428,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -493,7 +436,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -501,119 +444,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing before creating new branch
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>element</t>
   </si>
@@ -25,15 +25,57 @@
     <t>demand1</t>
   </si>
   <si>
+    <t>demand2</t>
+  </si>
+  <si>
     <t>net1</t>
   </si>
   <si>
+    <t>net2</t>
+  </si>
+  <si>
     <t>pv1</t>
   </si>
   <si>
+    <t>pv2</t>
+  </si>
+  <si>
     <t>bat1</t>
   </si>
   <si>
+    <t>bat2</t>
+  </si>
+  <si>
+    <t>CHP1</t>
+  </si>
+  <si>
+    <t>CHP2</t>
+  </si>
+  <si>
+    <t>solar_th1</t>
+  </si>
+  <si>
+    <t>solar_th2</t>
+  </si>
+  <si>
+    <t>pvt1</t>
+  </si>
+  <si>
+    <t>pvt2</t>
+  </si>
+  <si>
+    <t>charging_station1</t>
+  </si>
+  <si>
+    <t>charging_station2</t>
+  </si>
+  <si>
+    <t>heat_pump1</t>
+  </si>
+  <si>
+    <t>heat_pump2</t>
+  </si>
+  <si>
     <t>demand</t>
   </si>
   <si>
@@ -44,6 +86,21 @@
   </si>
   <si>
     <t>bat</t>
+  </si>
+  <si>
+    <t>CHP</t>
+  </si>
+  <si>
+    <t>solar_th</t>
+  </si>
+  <si>
+    <t>pvt</t>
+  </si>
+  <si>
+    <t>charging_station</t>
+  </si>
+  <si>
+    <t>heat_pump</t>
   </si>
 </sst>
 </file>
@@ -401,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -428,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -436,7 +493,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -444,7 +501,119 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test has important information
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>element</t>
   </si>
@@ -34,21 +34,6 @@
     <t>bat1</t>
   </si>
   <si>
-    <t>CHP1</t>
-  </si>
-  <si>
-    <t>solar_th1</t>
-  </si>
-  <si>
-    <t>pvt1</t>
-  </si>
-  <si>
-    <t>charging_station1</t>
-  </si>
-  <si>
-    <t>heat_pump1</t>
-  </si>
-  <si>
     <t>demand</t>
   </si>
   <si>
@@ -59,21 +44,6 @@
   </si>
   <si>
     <t>bat</t>
-  </si>
-  <si>
-    <t>CHP</t>
-  </si>
-  <si>
-    <t>solar_th</t>
-  </si>
-  <si>
-    <t>pvt</t>
-  </si>
-  <si>
-    <t>charging_station</t>
-  </si>
-  <si>
-    <t>heat_pump</t>
   </si>
 </sst>
 </file>
@@ -431,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -458,7 +428,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -466,7 +436,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -474,47 +444,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting before switching to main
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>element</t>
   </si>
@@ -25,82 +25,13 @@
     <t>demand1</t>
   </si>
   <si>
-    <t>demand2</t>
-  </si>
-  <si>
-    <t>net1</t>
-  </si>
-  <si>
-    <t>net2</t>
-  </si>
-  <si>
     <t>pv1</t>
   </si>
   <si>
-    <t>pv2</t>
-  </si>
-  <si>
-    <t>bat1</t>
-  </si>
-  <si>
-    <t>bat2</t>
-  </si>
-  <si>
-    <t>CHP1</t>
-  </si>
-  <si>
-    <t>CHP2</t>
-  </si>
-  <si>
-    <t>solar_th1</t>
-  </si>
-  <si>
-    <t>solar_th2</t>
-  </si>
-  <si>
-    <t>pvt1</t>
-  </si>
-  <si>
-    <t>pvt2</t>
-  </si>
-  <si>
-    <t>charging_station1</t>
-  </si>
-  <si>
-    <t>charging_station2</t>
-  </si>
-  <si>
-    <t>heat_pump1</t>
-  </si>
-  <si>
-    <t>heat_pump2</t>
-  </si>
-  <si>
     <t>demand</t>
   </si>
   <si>
-    <t>net</t>
-  </si>
-  <si>
     <t>pv</t>
-  </si>
-  <si>
-    <t>bat</t>
-  </si>
-  <si>
-    <t>CHP</t>
-  </si>
-  <si>
-    <t>solar_th</t>
-  </si>
-  <si>
-    <t>pvt</t>
-  </si>
-  <si>
-    <t>charging_station</t>
-  </si>
-  <si>
-    <t>heat_pump</t>
   </si>
 </sst>
 </file>
@@ -458,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,7 +408,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -485,135 +416,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MILESTONE a lot of changes
description in classes, binary in some classes, right values for maintenance and others
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>element</t>
   </si>
@@ -25,15 +25,9 @@
     <t>demand1</t>
   </si>
   <si>
-    <t>demand2</t>
-  </si>
-  <si>
     <t>net1</t>
   </si>
   <si>
-    <t>net2</t>
-  </si>
-  <si>
     <t>pv1</t>
   </si>
   <si>
@@ -76,6 +70,18 @@
     <t>heat_pump2</t>
   </si>
   <si>
+    <t>bat_with_aging1</t>
+  </si>
+  <si>
+    <t>bat_with_aging2</t>
+  </si>
+  <si>
+    <t>gas_boiler1</t>
+  </si>
+  <si>
+    <t>gas_boiler2</t>
+  </si>
+  <si>
     <t>demand</t>
   </si>
   <si>
@@ -101,6 +107,12 @@
   </si>
   <si>
     <t>heat_pump</t>
+  </si>
+  <si>
+    <t>bat_with_aging</t>
+  </si>
+  <si>
+    <t>gas_boiler</t>
   </si>
 </sst>
 </file>
@@ -458,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,7 +489,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -485,7 +497,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -493,7 +505,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -501,7 +513,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -509,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -517,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -525,7 +537,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -533,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -541,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -549,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -557,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -565,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -573,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -581,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -589,7 +601,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -597,7 +609,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -605,7 +617,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -613,7 +625,23 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
function that creates charts implemented
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>element</t>
   </si>
@@ -31,9 +31,6 @@
     <t>pv1</t>
   </si>
   <si>
-    <t>pv2</t>
-  </si>
-  <si>
     <t>bat1</t>
   </si>
   <si>
@@ -43,33 +40,15 @@
     <t>CHP1</t>
   </si>
   <si>
-    <t>CHP2</t>
-  </si>
-  <si>
     <t>solar_th1</t>
   </si>
   <si>
-    <t>solar_th2</t>
-  </si>
-  <si>
     <t>pvt1</t>
   </si>
   <si>
-    <t>pvt2</t>
-  </si>
-  <si>
-    <t>charging_station1</t>
-  </si>
-  <si>
-    <t>charging_station2</t>
-  </si>
-  <si>
     <t>heat_pump1</t>
   </si>
   <si>
-    <t>heat_pump2</t>
-  </si>
-  <si>
     <t>bat_with_aging1</t>
   </si>
   <si>
@@ -79,9 +58,6 @@
     <t>gas_boiler1</t>
   </si>
   <si>
-    <t>gas_boiler2</t>
-  </si>
-  <si>
     <t>demand</t>
   </si>
   <si>
@@ -101,9 +77,6 @@
   </si>
   <si>
     <t>pvt</t>
-  </si>
-  <si>
-    <t>charging_station</t>
   </si>
   <si>
     <t>heat_pump</t>
@@ -470,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -497,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -505,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -513,7 +486,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -521,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -529,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -537,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -545,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -553,7 +526,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -561,7 +534,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -569,7 +542,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -577,71 +550,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHP and heat_pump linearized
</commit_message>
<xml_diff>
--- a/output/df_aux.xlsx
+++ b/output/df_aux.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>element</t>
   </si>
@@ -34,30 +34,12 @@
     <t>bat1</t>
   </si>
   <si>
-    <t>bat2</t>
-  </si>
-  <si>
     <t>CHP1</t>
   </si>
   <si>
-    <t>solar_th1</t>
-  </si>
-  <si>
-    <t>pvt1</t>
-  </si>
-  <si>
     <t>heat_pump1</t>
   </si>
   <si>
-    <t>bat_with_aging1</t>
-  </si>
-  <si>
-    <t>bat_with_aging2</t>
-  </si>
-  <si>
-    <t>gas_boiler1</t>
-  </si>
-  <si>
     <t>demand</t>
   </si>
   <si>
@@ -73,19 +55,7 @@
     <t>CHP</t>
   </si>
   <si>
-    <t>solar_th</t>
-  </si>
-  <si>
-    <t>pvt</t>
-  </si>
-  <si>
     <t>heat_pump</t>
-  </si>
-  <si>
-    <t>bat_with_aging</t>
-  </si>
-  <si>
-    <t>gas_boiler</t>
   </si>
 </sst>
 </file>
@@ -443,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,7 +432,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -470,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -478,7 +448,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -486,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -494,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -502,55 +472,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
         <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>